<commit_message>
update from ci build
</commit_message>
<xml_diff>
--- a/StructureDefinition-be-allergyintolerance.xlsx
+++ b/StructureDefinition-be-allergyintolerance.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$40</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="311">
   <si>
     <t>Path</t>
   </si>
@@ -388,7 +388,8 @@
     <t>active | inactive | resolved</t>
   </si>
   <si>
-    <t>The clinical status of the allergy or intolerance.</t>
+    <t>The clinical status of the allergy or intolerance.
+When available, a provider SHOULD include it. When given, a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>Refer to [discussion](http://hl7.org/fhir/R4/extensibility.html#Special-Case) if clincalStatus is missing data.
@@ -398,6 +399,9 @@
     <t>required</t>
   </si>
   <si>
+    <t>The clinical status of the allergy or intolerance.</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/ValueSet/allergyintolerance-clinical|4.0.1</t>
   </si>
   <si>
@@ -417,7 +421,8 @@
     <t>unconfirmed | confirmed | refuted | entered-in-error</t>
   </si>
   <si>
-    <t>Assertion about certainty associated with the propensity, or potential risk, of a reaction to the identified substance (including pharmaceutical product).</t>
+    <t>Assertion about certainty associated with the propensity, or potential risk, of a reaction to the identified substance (including pharmaceutical product).
+When available, a provider SHOULD include it. When given, a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>The data type is CodeableConcept because verificationStatus has some clinical judgment involved, such that there might need to be more specificity than the required FHIR value set allows. For example, a SNOMED coding might allow for additional specificity.</t>
@@ -442,7 +447,8 @@
     <t>allergy | intolerance - Underlying mechanism (if known)</t>
   </si>
   <si>
-    <t>Identification of the underlying physiological mechanism for the reaction risk.</t>
+    <t>Identification of the underlying physiological mechanism for the reaction risk.
+When available, a provider SHOULD include it. When given, a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>Allergic (typically immune-mediated) reactions have been traditionally regarded as an indicator for potential escalation to significant future risk. Contemporary knowledge suggests that some reactions previously thought to be immune-mediated are, in fact, non-immune, but in some cases can still pose a life threatening risk. It is acknowledged that many clinicians might not be in a position to distinguish the mechanism of a particular reaction. Often the term "allergy" is used rather generically and may overlap with the use of "intolerance" - in practice the boundaries between these two concepts might not be well-defined or understood. This data element is included nevertheless, because many legacy systems have captured this attribute. Immunologic testing may provide supporting evidence for the basis of the reaction and the causative substance, but no tests are 100% sensitive or specific for sensitivity to a particular substance. If, as is commonly the case, it is unclear whether the reaction is due to an allergy or an intolerance, then the type element should be omitted from the resource.</t>
@@ -473,7 +479,8 @@
     <t>food | medication | environment | biologic</t>
   </si>
   <si>
-    <t>Category of the identified substance.</t>
+    <t>Category of the identified substance.
+When available, a provider SHOULD include it in the istance. When given, a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>This data element has been included because it is currently being captured in some clinical systems. This data can be derived from the substance where coding systems are used, and is effectively redundant in that situation.  When searching on category, consider the implications of AllergyIntolerance resources without a category.  For example, when searching on category = medication, medication allergies that don't have a category valued will not be returned.  Refer to [search](http://hl7.org/fhir/R4/search.html) for more information on how to search category with a :missing modifier to get allergies that don't have a category.  Additionally, category should be used with caution because category can be subjective based on the sender.</t>
@@ -532,7 +539,8 @@
     <t>Code that identifies the allergy or intolerance</t>
   </si>
   <si>
-    <t>Code for an allergy or intolerance statement (either a positive or a negated/excluded statement).  This may be a code for a substance or pharmaceutical product that is considered to be responsible for the adverse reaction risk (e.g., "Latex"), an allergy or intolerance condition (e.g., "Latex allergy"), or a negated/excluded code for a specific substance or class (e.g., "No latex allergy") or a general or categorical negated statement (e.g.,  "No known allergy", "No known drug allergies").  Note: the substance for a specific reaction may be different from the substance identified as the cause of the risk, but it must be consistent with it. For instance, it may be a more specific substance (e.g. a brand medication) or a composite product that includes the identified substance. It must be clinically safe to only process the 'code' and ignore the 'reaction.substance'.  If a receiving system is unable to confirm that AllergyIntolerance.reaction.substance falls within the semantic scope of AllergyIntolerance.code, then the receiving system should ignore AllergyIntolerance.reaction.substance.</t>
+    <t>Code for an allergy or intolerance statement (either a positive or a negated/excluded statement).  This may be a code for a substance or pharmaceutical product that is considered to be responsible for the adverse reaction risk (e.g., "Latex"), an allergy or intolerance condition (e.g., "Latex allergy"), or a negated/excluded code for a specific substance or class (e.g., "No latex allergy") or a general or categorical negated statement (e.g.,  "No known allergy", "No known drug allergies").  Note: the substance for a specific reaction may be different from the substance identified as the cause of the risk, but it must be consistent with it. For instance, it may be a more specific substance (e.g. a brand medication) or a composite product that includes the identified substance. It must be clinically safe to only process the 'code' and ignore the 'reaction.substance'.  If a receiving system is unable to confirm that AllergyIntolerance.reaction.substance falls within the semantic scope of AllergyIntolerance.code, then the receiving system should ignore AllergyIntolerance.reaction.substance.
+A provider SHALL include it in the istance and a consumer SHALL record this in its consuming system.  If needed codes can be used outside the given valueset, SNOMED-CT is preferred.</t>
   </si>
   <si>
     <t>It is strongly recommended that this element be populated using a terminology, where possible. For example, some terminologies used include RxNorm, SNOMED CT, DM+D, NDFRT, ICD-9, IDC-10, UNII, and ATC. Plain text should only be used if there is no appropriate terminology available. Additional details can be specified in the text.@@ -548,7 +556,7 @@
     <t>Causative agent codes as defined by NIHDI</t>
   </si>
   <si>
-    <t>https://www.ehealth.fgov.be/standards/fhir/ValueSet/be-causativeagent</t>
+    <t>https://www.ehealth.fgov.be/standards/fhir/ValueSet/be-allergyintolerancecode</t>
   </si>
   <si>
     <t>substance/product:@@ -584,7 +592,8 @@
     <t>Who the sensitivity is for</t>
   </si>
   <si>
-    <t>The patient who has the allergy or intolerance.</t>
+    <t>The patient who has the allergy or intolerance.
+A provider SHALL include it in the istance and a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>.participation[typeCode=SBJ].role[classCode=PAT]</t>
@@ -644,7 +653,8 @@
     <t>Date first version of the resource instance was recorded</t>
   </si>
   <si>
-    <t>The recordedDate represents when this particular AllergyIntolerance record was created in the system, which is often a system-generated date.</t>
+    <t>The recordedDate represents when this particular AllergyIntolerance record was created in the system, which is often a system-generated date.
+A provider SHALL include it in the istance and a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>.participation[typeCode=AUT].time</t>
@@ -663,14 +673,20 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(RelatedPerson|https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-patient|https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-practitioner|https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-practitionerrole)
+    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Patient|RelatedPerson|https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-patient|https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-practitioner|https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-practitionerrole)
 </t>
   </si>
   <si>
     <t>Who recorded the sensitivity</t>
   </si>
   <si>
-    <t>Individual who recorded the record and takes responsibility for its content.</t>
+    <t>Individual who recorded the record and takes responsibility for its content.
+A provider SHALL include it in the istance and a consumer SHALL record this in its consuming system.</t>
+  </si>
+  <si>
+    <t>References SHALL be a reference to an actual FHIR resource, and SHALL be resolveable (allowing for access control, temporary unavailability, etc.). Resolution can be either by retrieval from the URL, or, where applicable by resource type, by treating an absolute reference as a canonical URL and looking it up in a local registry/repository.
+Special remarks for KMEHR users:
+This is the 'author' concept in a KMEHR message as the FHIR recorder is the party taking responsibility.</t>
   </si>
   <si>
     <t>.participation[typeCode=AUT].role</t>
@@ -686,13 +702,20 @@
 Informant</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference(Patient|RelatedPerson|Practitioner|PractitionerRole)
+</t>
+  </si>
+  <si>
     <t>Source of the information about the allergy</t>
   </si>
   <si>
-    <t>The source of the information about the allergy that is recorded.</t>
-  </si>
-  <si>
-    <t>The recorder takes responsibility for the content, but can reference the source from where they got it.</t>
+    <t>The source of the information about the allergy that is recorded.
+When available, a provider SHOULD include it in the istance. When given, a consumer SHALL record this in its consuming system.</t>
+  </si>
+  <si>
+    <t>The recorder takes responsibility for the content, but can reference the source from where they got it.
+Special remarks for KMEHR users:
+As the FHIR asserter is not the party taking responsibility, this is not equal to the 'author' concept in KMEHR.</t>
   </si>
   <si>
     <t>.participation[typeCode=INF].role</t>
@@ -732,7 +755,8 @@
     <t>Additional narrative about the propensity for the Adverse Reaction, not captured in other fields.</t>
   </si>
   <si>
-    <t>For example: including reason for flagging a seriousness of 'High Risk'; and instructions related to future exposure or administration of the substance, such as administration within an Intensive Care Unit or under corticosteroid cover. The notes should be related to an allergy or intolerance as a condition in general and not related to any particular episode of it. For episode notes and descriptions, use AllergyIntolerance.event.description and  AllergyIntolerance.event.notes.</t>
+    <t>For example: including reason for flagging a seriousness of 'High Risk'; and instructions related to future exposure or administration of the substance, such as administration within an Intensive Care Unit or under corticosteroid cover. The notes should be related to an allergy or intolerance as a condition in general and not related to any particular episode of it. For episode notes and descriptions, use AllergyIntolerance.event.description and  AllergyIntolerance.event.notes.
+When available, a provider SHOULD include it. When given, a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>subjectOf.observationEvent[code="annotation"].value</t>
@@ -748,7 +772,8 @@
     <t>Adverse Reaction Events linked to exposure to substance</t>
   </si>
   <si>
-    <t>Details about each adverse reaction event linked to exposure to the identified substance.</t>
+    <t>Details about each adverse reaction event linked to exposure to the identified substance.
+When available, a provider SHOULD include it in the istance. When given, a consumer SHALL record this in its consuming system.</t>
   </si>
   <si>
     <t>outBoundRelationship[typeCode=SUBJ].target[classCode=OBS, moodCode=EVN, code &lt;= CommonClinicalObservationType, value &lt;= ObservationValue (Reaction Type)]</t>
@@ -829,7 +854,8 @@
     <t>Clinical symptoms/signs associated with the Event</t>
   </si>
   <si>
-    <t>Clinical symptoms and/or signs that are observed or associated with the adverse reaction event.</t>
+    <t>Clinical symptoms and/or signs that are observed or associated with the adverse reaction event.
+When available, a provider SHOULD include it. When given, a consumer SHALL record this in its consuming system. If needed codes can be used outside the given valueset, SNOMED-CT is preferred.</t>
   </si>
   <si>
     <t>Manifestation can be expressed as a single word, phrase or brief description. For example: nausea, rash or no reaction. It is preferable that manifestation should be coded with a terminology, where possible. The values entered here may be used to display on an application screen as part of a list of adverse reactions, as recommended in the UK NHS CUI guidelines.  Terminologies commonly used include, but are not limited to, SNOMED CT or ICD10.</t>
@@ -896,7 +922,7 @@
     <t>How the subject was exposed to the substance</t>
   </si>
   <si>
-    <t>Identification of the route by which the subject was exposed to the substance.</t>
+    <t>Identification of the route by which the subject was exposed to the substance.  If needed codes can be used outside the given valueset, SNOMED-CT is preferred.</t>
   </si>
   <si>
     <t>Coding of the route of exposure with a terminology should be used wherever possible.</t>
@@ -911,13 +937,85 @@
     <t>outBoundRelationship[typeCode=SAS].target[classCode=SBADM, code &lt;= ExposureCode].routeCode</t>
   </si>
   <si>
+    <t>AllergyIntolerance.reaction.exposureRoute.id</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.reaction.exposureRoute.extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.reaction.exposureRoute.coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding
+</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>https://www.ehealth.fgov.be/standards/fhir/ValueSet/be-exposureroute</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.reaction.exposureRoute.text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
     <t>AllergyIntolerance.reaction.note</t>
   </si>
   <si>
     <t>Text about event not captured in other fields</t>
   </si>
   <si>
-    <t>Additional text about the adverse reaction event not captured in other fields.</t>
+    <t>Additional text about the adverse reaction event not captured in other fields.
+A note on this level SHOULD be avoided when not absolutely necessary. Preferably use the .note one level higher.</t>
   </si>
   <si>
     <t>Use this field to record information indirectly related to a particular event and not captured in the description. For example: Clinical records are no longer available, recorded based on information provided to the patient by her mother and her mother is deceased.</t>
@@ -1069,7 +1167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL36"/>
+  <dimension ref="A1:AL40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1078,7 +1176,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.24609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="48.7890625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -1102,10 +1200,10 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="120.87890625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="68.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="73.83984375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="39.515625" customWidth="true" bestFit="true" hidden="true"/>
@@ -1115,7 +1213,7 @@
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="255.0" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="40.12109375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="43.9296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2379,10 +2477,10 @@
         <v>120</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>42</v>
@@ -2409,16 +2507,16 @@
         <v>49</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AI12" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>42</v>
@@ -2426,7 +2524,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2452,13 +2550,13 @@
         <v>116</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -2487,10 +2585,10 @@
         <v>120</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>42</v>
@@ -2508,7 +2606,7 @@
         <v>42</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>40</v>
@@ -2517,16 +2615,16 @@
         <v>49</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AI13" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>42</v>
@@ -2534,11 +2632,11 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -2560,13 +2658,13 @@
         <v>69</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2595,10 +2693,10 @@
         <v>120</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>42</v>
@@ -2616,7 +2714,7 @@
         <v>42</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>40</v>
@@ -2631,22 +2729,22 @@
         <v>61</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -2668,13 +2766,13 @@
         <v>69</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -2703,10 +2801,10 @@
         <v>120</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>42</v>
@@ -2724,7 +2822,7 @@
         <v>42</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
@@ -2739,22 +2837,22 @@
         <v>61</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -2776,13 +2874,13 @@
         <v>69</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2811,10 +2909,10 @@
         <v>120</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>42</v>
@@ -2832,7 +2930,7 @@
         <v>42</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>40</v>
@@ -2847,22 +2945,22 @@
         <v>61</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -2872,7 +2970,7 @@
         <v>49</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>42</v>
@@ -2884,13 +2982,13 @@
         <v>116</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -2916,13 +3014,13 @@
         <v>42</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>42</v>
@@ -2940,7 +3038,7 @@
         <v>42</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
@@ -2955,22 +3053,22 @@
         <v>61</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -2989,13 +3087,13 @@
         <v>50</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3046,7 +3144,7 @@
         <v>42</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>49</v>
@@ -3061,18 +3159,18 @@
         <v>61</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3095,13 +3193,13 @@
         <v>42</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3152,7 +3250,7 @@
         <v>42</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -3167,10 +3265,10 @@
         <v>61</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>42</v>
@@ -3178,7 +3276,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3201,13 +3299,13 @@
         <v>42</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3258,7 +3356,7 @@
         <v>42</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
@@ -3273,10 +3371,10 @@
         <v>61</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>42</v>
@@ -3284,7 +3382,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3307,13 +3405,13 @@
         <v>42</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3364,7 +3462,7 @@
         <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3379,22 +3477,22 @@
         <v>61</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -3413,15 +3511,17 @@
         <v>42</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="M22" s="2"/>
+        <v>204</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>205</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>42</v>
@@ -3470,7 +3570,7 @@
         <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3485,10 +3585,10 @@
         <v>61</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>42</v>
@@ -3496,11 +3596,11 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3519,16 +3619,16 @@
         <v>50</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -3578,7 +3678,7 @@
         <v>42</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -3593,18 +3693,18 @@
         <v>61</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3627,16 +3727,16 @@
         <v>42</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3686,7 +3786,7 @@
         <v>42</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3701,7 +3801,7 @@
         <v>61</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>42</v>
@@ -3712,7 +3812,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3735,16 +3835,16 @@
         <v>42</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3794,7 +3894,7 @@
         <v>42</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -3809,7 +3909,7 @@
         <v>61</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>42</v>
@@ -3820,7 +3920,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3843,13 +3943,13 @@
         <v>42</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -3900,7 +4000,7 @@
         <v>42</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
@@ -3915,7 +4015,7 @@
         <v>61</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>42</v>
@@ -3926,7 +4026,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3952,10 +4052,10 @@
         <v>51</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4006,7 +4106,7 @@
         <v>42</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
@@ -4021,7 +4121,7 @@
         <v>42</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>42</v>
@@ -4032,7 +4132,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4061,7 +4161,7 @@
         <v>96</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="M28" t="s" s="2">
         <v>98</v>
@@ -4114,7 +4214,7 @@
         <v>42</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
@@ -4129,7 +4229,7 @@
         <v>100</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>42</v>
@@ -4140,11 +4240,11 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
@@ -4166,10 +4266,10 @@
         <v>95</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="M29" t="s" s="2">
         <v>98</v>
@@ -4224,7 +4324,7 @@
         <v>42</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4248,9 +4348,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4264,7 +4364,7 @@
         <v>49</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>42</v>
@@ -4276,13 +4376,13 @@
         <v>116</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4308,13 +4408,13 @@
         <v>42</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>42</v>
@@ -4332,7 +4432,7 @@
         <v>42</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
@@ -4347,7 +4447,7 @@
         <v>61</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>42</v>
@@ -4358,11 +4458,11 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -4384,13 +4484,13 @@
         <v>116</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4416,11 +4516,11 @@
         <v>42</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="X31" s="2"/>
       <c r="Y31" t="s" s="2">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>42</v>
@@ -4438,7 +4538,7 @@
         <v>42</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>49</v>
@@ -4453,22 +4553,22 @@
         <v>61</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -4490,13 +4590,13 @@
         <v>51</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4546,7 +4646,7 @@
         <v>42</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
@@ -4561,7 +4661,7 @@
         <v>61</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>42</v>
@@ -4570,9 +4670,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4586,7 +4686,7 @@
         <v>49</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>42</v>
@@ -4595,13 +4695,13 @@
         <v>42</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -4652,7 +4752,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -4667,18 +4767,18 @@
         <v>61</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4704,13 +4804,13 @@
         <v>69</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -4739,10 +4839,10 @@
         <v>120</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>42</v>
@@ -4760,7 +4860,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -4775,7 +4875,7 @@
         <v>61</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>42</v>
@@ -4786,7 +4886,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4812,13 +4912,13 @@
         <v>116</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -4844,13 +4944,13 @@
         <v>42</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>42</v>
@@ -4868,7 +4968,7 @@
         <v>42</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
@@ -4883,7 +4983,7 @@
         <v>61</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>42</v>
@@ -4892,9 +4992,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4905,10 +5005,10 @@
         <v>40</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>42</v>
@@ -4917,17 +5017,15 @@
         <v>42</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>282</v>
+        <v>234</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>284</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>42</v>
@@ -4976,32 +5074,466 @@
         <v>42</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG36" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="AK36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL36" t="s" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" hidden="true">
+      <c r="A37" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F37" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AH36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI36" t="s" s="2">
+      <c r="G37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="N37" s="2"/>
+      <c r="O37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P37" s="2"/>
+      <c r="Q37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA37" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD37" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AE37" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AF37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI37" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL37" t="s" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" hidden="true">
+      <c r="A38" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I38" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="J38" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="K38" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="N38" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="O38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P38" s="2"/>
+      <c r="Q38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W38" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="X38" s="2"/>
+      <c r="Y38" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="Z38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE38" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="AF38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI38" t="s" s="2">
         <v>61</v>
       </c>
-      <c r="AJ36" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AJ38" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL38" t="s" s="2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="39" hidden="true">
+      <c r="A39" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F39" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I39" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="J39" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="K39" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="L39" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="O39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P39" s="2"/>
+      <c r="Q39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE39" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="AF39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI39" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AK39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL39" t="s" s="2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" hidden="true">
+      <c r="A40" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="J40" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="N40" s="2"/>
+      <c r="O40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P40" s="2"/>
+      <c r="Q40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL36">
+  <autoFilter ref="A1:AL40">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5011,7 +5543,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI35">
+  <conditionalFormatting sqref="A2:AI39">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>